<commit_message>
1st runnable version using  simplified_data1
</commit_message>
<xml_diff>
--- a/simplified_data/simplified_1.xlsx
+++ b/simplified_data/simplified_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taliah\code\ml_class\tcm-project\ml-tcm-nn\ML_TCM_NN\simplified_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9CEBFE-1270-43EE-AC67-FFBA06C36887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5DA9768-6129-4583-AE36-1840987788D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{2A006EB1-B134-4D0E-8B65-59B8103F3B09}"/>
   </bookViews>
@@ -1467,11 +1467,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47BB0B2B-BA7D-486B-AEF4-0F8186B490F3}">
   <dimension ref="A1:GK116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="FL1" workbookViewId="0">
+      <selection activeCell="ER14" sqref="ER14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="95.75" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:193" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>